<commit_message>
Update All Master Data role Admin
</commit_message>
<xml_diff>
--- a/public/assets/template/peminatan.xlsx
+++ b/public/assets/template/peminatan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\pipe\public\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pipe\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8D5079-ED05-4114-853A-BD699985F619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC815450-88A5-491F-9089-90979C888CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>kelompok</t>
-  </si>
-  <si>
-    <t>peminatan</t>
-  </si>
-  <si>
-    <t>Nama Dosen</t>
-  </si>
-  <si>
-    <t>Kelompok Peminatan</t>
-  </si>
-  <si>
-    <t>Peminatan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>kodepeminatan</t>
+  </si>
+  <si>
+    <t>Kode Peminatan</t>
+  </si>
+  <si>
+    <t>namapeminatan</t>
+  </si>
+  <si>
+    <t>Nama Peminatan</t>
+  </si>
+  <si>
+    <t>kelompokkeahlian</t>
+  </si>
+  <si>
+    <t>Kelompok Keahlian</t>
+  </si>
+  <si>
+    <t>kuota</t>
+  </si>
+  <si>
+    <t>Kuota</t>
   </si>
 </sst>
 </file>
@@ -360,34 +366,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template excel peminatan dan keprof
</commit_message>
<xml_diff>
--- a/public/assets/template/peminatan.xlsx
+++ b/public/assets/template/peminatan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pipe\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC815450-88A5-491F-9089-90979C888CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BD3F65-F07F-4B55-AD30-BD09AF671448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,11 +384,11 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -398,7 +398,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>